<commit_message>
All xml for more estimates
</commit_message>
<xml_diff>
--- a/src/test/resources/Documents/3965/Actual/JobMaterial.xlsx
+++ b/src/test/resources/Documents/3965/Actual/JobMaterial.xlsx
@@ -68,6 +68,9 @@
     <t>M594GN - 4/C Process (General)</t>
   </si>
   <si>
+    <t xml:space="preserve">Magenta - Sheet-fed Offset - </t>
+  </si>
+  <si>
     <t xml:space="preserve">Yellow - Sheet-fed Offset - </t>
   </si>
   <si>
@@ -75,9 +78,6 @@
   </si>
   <si>
     <t>M594GK - Black (General)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magenta - Sheet-fed Offset - </t>
   </si>
   <si>
     <t>Plate</t>
@@ -649,7 +649,7 @@
         <v>16</v>
       </c>
       <c r="H4" t="s" s="29">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s" s="30">
         <v>16</v>
@@ -669,7 +669,7 @@
         <v>12</v>
       </c>
       <c r="D5" t="s" s="35">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s" s="36">
         <v>14</v>
@@ -681,7 +681,7 @@
         <v>16</v>
       </c>
       <c r="H5" t="s" s="39">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I5" t="s" s="40">
         <v>16</v>

</xml_diff>